<commit_message>
Categorise ranking table csv.
</commit_message>
<xml_diff>
--- a/demo/data/ResumeTemplate_keys.xlsx
+++ b/demo/data/ResumeTemplate_keys.xlsx
@@ -1097,13 +1097,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J464"/>
+  <dimension ref="A1:J566"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
     <col width="18.5545454545455" customWidth="1" min="1" max="1"/>
     <col width="26.3636363636364" customWidth="1" min="2" max="2"/>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>joined cognizant- dec</t>
+          <t>april</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>programmer analyst trainee</t>
+          <t>till</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>dec</t>
+          <t>amgen</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -1523,7 +1523,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>march</t>
+          <t>programmer analyst</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>trained</t>
+          <t>around</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1627,7 +1627,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>cognizant</t>
+          <t>strong relationship</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1679,7 +1679,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>advanced java</t>
+          <t>end users</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1731,7 +1731,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>coimbatore</t>
+          <t>technical resources</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1783,7 +1783,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>april</t>
+          <t>installation</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1820,7 +1820,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>till</t>
+          <t>management</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1857,7 +1857,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>amgen</t>
+          <t>various web applications</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1889,7 +1889,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>programmer analyst</t>
+          <t>ensure</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1921,7 +1921,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>around</t>
+          <t>overall organizational support goals</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>strong relationship</t>
+          <t>sla</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1975,7 +1975,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>end users</t>
+          <t>incident / problem reduction</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -2002,7 +2002,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>technical resources applications</t>
+          <t>functional skills</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -2029,7 +2029,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>installation</t>
+          <t>itil processes it infrastructure support intense</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -2056,7 +2056,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>management</t>
+          <t>passionate</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -2083,7 +2083,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>various web applications</t>
+          <t>customer focus </t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -2110,7 +2110,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>functional skills</t>
+          <t>thoughtful</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2132,7 +2132,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>itil processes it infrastructure support intense</t>
+          <t>execution </t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2154,7 +2154,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>passionate</t>
+          <t>tenacious</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2176,7 +2176,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>customer focus </t>
+          <t>continuous improvement </t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2198,7 +2198,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>thoughtful</t>
+          <t>relentless</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -2220,7 +2220,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>execution </t>
+          <t>understanding</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -2242,7 +2242,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>tenacious</t>
+          <t>user requirements</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -2264,7 +2264,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>continuous improvement </t>
+          <t>bug</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -2286,7 +2286,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>relentless</t>
+          <t>business problems</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -2308,7 +2308,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>understanding</t>
+          <t>new technologies / process</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -2330,7 +2330,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>user requirements</t>
+          <t>customer satisfaction</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -2352,7 +2352,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>bug</t>
+          <t>technical components</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -2374,7 +2374,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>business problems</t>
+          <t>abe</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -2396,7 +2396,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>new technologies / process</t>
+          <t>it projects</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -2418,7 +2418,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>customer satisfaction</t>
+          <t>concepts</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
@@ -2440,7 +2440,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>technical components</t>
+          <t>programming</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
@@ -2462,7 +2462,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>abe</t>
+          <t>it support</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -2484,7 +2484,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>it projects</t>
+          <t>technologies</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>concepts</t>
+          <t>unix</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
@@ -2528,7 +2528,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>programming</t>
+          <t>c++</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -2550,7 +2550,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>it support technical skills</t>
+          <t>windows</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
@@ -2572,7 +2572,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>technologies</t>
+          <t>linux</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -2589,7 +2589,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>unix</t>
+          <t>pursuing</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -2606,7 +2606,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>c++</t>
+          <t>confluence</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
@@ -2623,7 +2623,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>windows</t>
+          <t>shared repository</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -2640,7 +2640,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>linux</t>
+          <t>concur travel app</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -2657,7 +2657,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>pursuing</t>
+          <t>tangoe payment</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
@@ -2674,7 +2674,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>confluence</t>
+          <t>files  service</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
@@ -2691,7 +2691,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>shared repository</t>
+          <t>informatica</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
@@ -2708,7 +2708,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>concur travel app</t>
+          <t>oracle sql</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
@@ -2725,7 +2725,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>tangoe payment</t>
+          <t>developer </t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
@@ -2742,7 +2742,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>files  service</t>
+          <t>jxplorer</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
@@ -2759,7 +2759,7 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>informatica</t>
+          <t>tortoise svn</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
@@ -2776,7 +2776,7 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>oracle sql</t>
+          <t>dec</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
@@ -2793,7 +2793,7 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>developer </t>
+          <t>march</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
@@ -2810,7 +2810,7 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>jxplorer</t>
+          <t>trained</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
@@ -2822,7 +2822,7 @@
     <row r="60">
       <c r="I60" t="inlineStr">
         <is>
-          <t>tortoise svn</t>
+          <t>cognizant</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
@@ -2834,7 +2834,7 @@
     <row r="61">
       <c r="I61" t="inlineStr">
         <is>
-          <t>location</t>
+          <t>advanced java</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
@@ -2846,7 +2846,7 @@
     <row r="62">
       <c r="I62" t="inlineStr">
         <is>
-          <t>chennai</t>
+          <t>coimbatore</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="63">
       <c r="I63" t="inlineStr">
         <is>
-          <t>india integration</t>
+          <t>location</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
@@ -2870,7 +2870,7 @@
     <row r="64">
       <c r="I64" t="inlineStr">
         <is>
-          <t>various tools</t>
+          <t>chennai</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
@@ -2882,7 +2882,7 @@
     <row r="65">
       <c r="I65" t="inlineStr">
         <is>
-          <t>prism</t>
+          <t>india</t>
         </is>
       </c>
       <c r="J65" t="inlineStr">
@@ -2894,7 +2894,7 @@
     <row r="66">
       <c r="I66" t="inlineStr">
         <is>
-          <t>rally</t>
+          <t>web</t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
@@ -2906,7 +2906,7 @@
     <row r="67">
       <c r="I67" t="inlineStr">
         <is>
-          <t>jira</t>
+          <t>logic upgrade –</t>
         </is>
       </c>
       <c r="J67" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="68">
       <c r="I68" t="inlineStr">
         <is>
-          <t>server deployments</t>
+          <t>version upgrade</t>
         </is>
       </c>
       <c r="J68" t="inlineStr">
@@ -2930,7 +2930,7 @@
     <row r="69">
       <c r="I69" t="inlineStr">
         <is>
-          <t>ownership-</t>
+          <t>minor enhancements</t>
         </is>
       </c>
       <c r="J69" t="inlineStr">
@@ -2942,7 +2942,7 @@
     <row r="70">
       <c r="I70" t="inlineStr">
         <is>
-          <t>system owner</t>
+          <t>jira</t>
         </is>
       </c>
       <c r="J70" t="inlineStr">
@@ -2954,7 +2954,7 @@
     <row r="71">
       <c r="I71" t="inlineStr">
         <is>
-          <t>role</t>
+          <t>various tools</t>
         </is>
       </c>
       <c r="J71" t="inlineStr">
@@ -2966,7 +2966,7 @@
     <row r="72">
       <c r="I72" t="inlineStr">
         <is>
-          <t>cognizant part</t>
+          <t>prism</t>
         </is>
       </c>
       <c r="J72" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="73">
       <c r="I73" t="inlineStr">
         <is>
-          <t>svn</t>
+          <t>rally</t>
         </is>
       </c>
       <c r="J73" t="inlineStr">
@@ -2990,7 +2990,7 @@
     <row r="74">
       <c r="I74" t="inlineStr">
         <is>
-          <t>tangoe</t>
+          <t>various teams</t>
         </is>
       </c>
       <c r="J74" t="inlineStr">
@@ -3002,7 +3002,7 @@
     <row r="75">
       <c r="I75" t="inlineStr">
         <is>
-          <t>payment files</t>
+          <t>server deployments</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -3014,7 +3014,7 @@
     <row r="76">
       <c r="I76" t="inlineStr">
         <is>
-          <t>responsible/</t>
+          <t>svn</t>
         </is>
       </c>
       <c r="J76" t="inlineStr">
@@ -3026,7 +3026,7 @@
     <row r="77">
       <c r="I77" t="inlineStr">
         <is>
-          <t>above applications</t>
+          <t>tangoe</t>
         </is>
       </c>
       <c r="J77" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="78">
       <c r="I78" t="inlineStr">
         <is>
-          <t>cognizant end</t>
+          <t>payment files</t>
         </is>
       </c>
       <c r="J78" t="inlineStr">
@@ -3050,7 +3050,7 @@
     <row r="79">
       <c r="I79" t="inlineStr">
         <is>
-          <t>writing</t>
+          <t>responsible/</t>
         </is>
       </c>
       <c r="J79" t="inlineStr">
@@ -3062,7 +3062,7 @@
     <row r="80">
       <c r="I80" t="inlineStr">
         <is>
-          <t>standard tasks</t>
+          <t>above applications</t>
         </is>
       </c>
       <c r="J80" t="inlineStr">
@@ -3074,7 +3074,7 @@
     <row r="81">
       <c r="I81" t="inlineStr">
         <is>
-          <t>defect</t>
+          <t>cognizant end</t>
         </is>
       </c>
       <c r="J81" t="inlineStr">
@@ -3086,7 +3086,7 @@
     <row r="82">
       <c r="I82" t="inlineStr">
         <is>
-          <t>servers</t>
+          <t>writing</t>
         </is>
       </c>
       <c r="J82" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="83">
       <c r="I83" t="inlineStr">
         <is>
-          <t>disk utilization</t>
+          <t>standard tasks</t>
         </is>
       </c>
       <c r="J83" t="inlineStr">
@@ -3110,7 +3110,7 @@
     <row r="84">
       <c r="I84" t="inlineStr">
         <is>
-          <t>cpu utilization</t>
+          <t>collaborate</t>
         </is>
       </c>
       <c r="J84" t="inlineStr">
@@ -3122,7 +3122,7 @@
     <row r="85">
       <c r="I85" t="inlineStr">
         <is>
-          <t>memory utilization</t>
+          <t>technical teams</t>
         </is>
       </c>
       <c r="J85" t="inlineStr">
@@ -3134,7 +3134,7 @@
     <row r="86">
       <c r="I86" t="inlineStr">
         <is>
-          <t>monitoring</t>
+          <t>proper integration</t>
         </is>
       </c>
       <c r="J86" t="inlineStr">
@@ -3146,7 +3146,7 @@
     <row r="87">
       <c r="I87" t="inlineStr">
         <is>
-          <t>application process</t>
+          <t>defect</t>
         </is>
       </c>
       <c r="J87" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="88">
       <c r="I88" t="inlineStr">
         <is>
-          <t>application logs</t>
+          <t>servers</t>
         </is>
       </c>
       <c r="J88" t="inlineStr">
@@ -3170,7 +3170,7 @@
     <row r="89">
       <c r="I89" t="inlineStr">
         <is>
-          <t>appropriate resolutions</t>
+          <t>disk utilization</t>
         </is>
       </c>
       <c r="J89" t="inlineStr">
@@ -3182,7 +3182,7 @@
     <row r="90">
       <c r="I90" t="inlineStr">
         <is>
-          <t>data base</t>
+          <t>cpu utilization</t>
         </is>
       </c>
       <c r="J90" t="inlineStr">
@@ -3194,7 +3194,7 @@
     <row r="91">
       <c r="I91" t="inlineStr">
         <is>
-          <t>oracle sql developer tools used</t>
+          <t>memory utilization</t>
         </is>
       </c>
       <c r="J91" t="inlineStr">
@@ -3206,7 +3206,7 @@
     <row r="92">
       <c r="I92" t="inlineStr">
         <is>
-          <t>employment</t>
+          <t>monitoring</t>
         </is>
       </c>
       <c r="J92" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="I93" t="inlineStr">
         <is>
-          <t>project details</t>
+          <t>application process</t>
         </is>
       </c>
       <c r="J93" t="inlineStr">
@@ -3230,7 +3230,7 @@
     <row r="94">
       <c r="I94" t="inlineStr">
         <is>
-          <t>project title</t>
+          <t>application logs</t>
         </is>
       </c>
       <c r="J94" t="inlineStr">
@@ -3242,7 +3242,7 @@
     <row r="95">
       <c r="I95" t="inlineStr">
         <is>
-          <t>domain</t>
+          <t>appropriate resolutions</t>
         </is>
       </c>
       <c r="J95" t="inlineStr">
@@ -3254,7 +3254,7 @@
     <row r="96">
       <c r="I96" t="inlineStr">
         <is>
-          <t>life science </t>
+          <t>data base</t>
         </is>
       </c>
       <c r="J96" t="inlineStr">
@@ -3266,7 +3266,7 @@
     <row r="97">
       <c r="I97" t="inlineStr">
         <is>
-          <t>environment</t>
+          <t>oracle sql developer tools used</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="98">
       <c r="I98" t="inlineStr">
         <is>
-          <t>web</t>
+          <t>employment</t>
         </is>
       </c>
       <c r="J98" t="inlineStr">
@@ -3290,7 +3290,7 @@
     <row r="99">
       <c r="I99" t="inlineStr">
         <is>
-          <t>logic upgrade –</t>
+          <t>project details</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -3302,7 +3302,7 @@
     <row r="100">
       <c r="I100" t="inlineStr">
         <is>
-          <t>version upgrade</t>
+          <t>project title</t>
         </is>
       </c>
       <c r="J100" t="inlineStr">
@@ -3314,7 +3314,7 @@
     <row r="101">
       <c r="I101" t="inlineStr">
         <is>
-          <t>minor enhancements</t>
+          <t>domain</t>
         </is>
       </c>
       <c r="J101" t="inlineStr">
@@ -3326,7 +3326,7 @@
     <row r="102">
       <c r="I102" t="inlineStr">
         <is>
-          <t>improvement</t>
+          <t>life science </t>
         </is>
       </c>
       <c r="J102" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="103">
       <c r="I103" t="inlineStr">
         <is>
-          <t>various teams</t>
+          <t>role</t>
         </is>
       </c>
       <c r="J103" t="inlineStr">
@@ -3350,7 +3350,7 @@
     <row r="104">
       <c r="I104" t="inlineStr">
         <is>
-          <t>complex project</t>
+          <t>environment</t>
         </is>
       </c>
       <c r="J104" t="inlineStr">
@@ -3362,7 +3362,7 @@
     <row r="105">
       <c r="I105" t="inlineStr">
         <is>
-          <t>multiple appreciation</t>
+          <t>java improvement</t>
         </is>
       </c>
       <c r="J105" t="inlineStr">
@@ -3374,7 +3374,7 @@
     <row r="106">
       <c r="I106" t="inlineStr">
         <is>
-          <t>project management</t>
+          <t>complex project</t>
         </is>
       </c>
       <c r="J106" t="inlineStr">
@@ -3386,7 +3386,7 @@
     <row r="107">
       <c r="I107" t="inlineStr">
         <is>
-          <t>star performer award</t>
+          <t>multiple appreciation</t>
         </is>
       </c>
       <c r="J107" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="108">
       <c r="I108" t="inlineStr">
         <is>
-          <t>ensure</t>
+          <t>project management</t>
         </is>
       </c>
       <c r="J108" t="inlineStr">
@@ -3410,7 +3410,7 @@
     <row r="109">
       <c r="I109" t="inlineStr">
         <is>
-          <t>overall organizational support goals</t>
+          <t>star performer award</t>
         </is>
       </c>
       <c r="J109" t="inlineStr">
@@ -3422,7 +3422,7 @@
     <row r="110">
       <c r="I110" t="inlineStr">
         <is>
-          <t>sla</t>
+          <t>ensures</t>
         </is>
       </c>
       <c r="J110" t="inlineStr">
@@ -3434,7 +3434,7 @@
     <row r="111">
       <c r="I111" t="inlineStr">
         <is>
-          <t>incident / problem reduction</t>
+          <t>systems events</t>
         </is>
       </c>
       <c r="J111" t="inlineStr">
@@ -3446,7 +3446,7 @@
     <row r="112">
       <c r="I112" t="inlineStr">
         <is>
-          <t>application </t>
+          <t>summary</t>
         </is>
       </c>
       <c r="J112" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="113">
       <c r="I113" t="inlineStr">
         <is>
-          <t>collaborate</t>
+          <t> 14+ years</t>
         </is>
       </c>
       <c r="J113" t="inlineStr">
@@ -3470,7 +3470,7 @@
     <row r="114">
       <c r="I114" t="inlineStr">
         <is>
-          <t>technical teams</t>
+          <t>soa</t>
         </is>
       </c>
       <c r="J114" t="inlineStr">
@@ -3482,7 +3482,7 @@
     <row r="115">
       <c r="I115" t="inlineStr">
         <is>
-          <t>proper integration</t>
+          <t>uml</t>
         </is>
       </c>
       <c r="J115" t="inlineStr">
@@ -3494,7 +3494,7 @@
     <row r="116">
       <c r="I116" t="inlineStr">
         <is>
-          <t>ensures</t>
+          <t>patterns</t>
         </is>
       </c>
       <c r="J116" t="inlineStr">
@@ -3506,7 +3506,7 @@
     <row r="117">
       <c r="I117" t="inlineStr">
         <is>
-          <t>systems events</t>
+          <t>financial</t>
         </is>
       </c>
       <c r="J117" t="inlineStr">
@@ -3516,6 +3516,11 @@
       </c>
     </row>
     <row r="118">
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>domains</t>
+        </is>
+      </c>
       <c r="J118" t="inlineStr">
         <is>
           <t>database</t>
@@ -3523,6 +3528,11 @@
       </c>
     </row>
     <row r="119">
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>billing systems</t>
+        </is>
+      </c>
       <c r="J119" t="inlineStr">
         <is>
           <t>written soap</t>
@@ -3530,6 +3540,11 @@
       </c>
     </row>
     <row r="120">
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>extensive</t>
+        </is>
+      </c>
       <c r="J120" t="inlineStr">
         <is>
           <t>web services</t>
@@ -3537,6 +3552,11 @@
       </c>
     </row>
     <row r="121">
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>oriented architecture</t>
+        </is>
+      </c>
       <c r="J121" t="inlineStr">
         <is>
           <t>project name environment description</t>
@@ -3544,6 +3564,11 @@
       </c>
     </row>
     <row r="122">
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>systems design</t>
+        </is>
+      </c>
       <c r="J122" t="inlineStr">
         <is>
           <t>java developer festiot</t>
@@ -3551,6 +3576,11 @@
       </c>
     </row>
     <row r="123">
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>n-tier applications</t>
+        </is>
+      </c>
       <c r="J123" t="inlineStr">
         <is>
           <t>client requirement</t>
@@ -3558,6 +3588,11 @@
       </c>
     </row>
     <row r="124">
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>proven</t>
+        </is>
+      </c>
       <c r="J124" t="inlineStr">
         <is>
           <t>special request</t>
@@ -3565,6 +3600,11 @@
       </c>
     </row>
     <row r="125">
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>principles</t>
+        </is>
+      </c>
       <c r="J125" t="inlineStr">
         <is>
           <t xml:space="preserve">menus </t>
@@ -3572,6 +3612,11 @@
       </c>
     </row>
     <row r="126">
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>project life cycle experience</t>
+        </is>
+      </c>
       <c r="J126" t="inlineStr">
         <is>
           <t>involved</t>
@@ -3579,6 +3624,11 @@
       </c>
     </row>
     <row r="127">
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>sdlc</t>
+        </is>
+      </c>
       <c r="J127" t="inlineStr">
         <is>
           <t>scrum</t>
@@ -3586,6 +3636,11 @@
       </c>
     </row>
     <row r="128">
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>requirements specifications</t>
+        </is>
+      </c>
       <c r="J128" t="inlineStr">
         <is>
           <t>scrum meeting</t>
@@ -3593,6 +3648,11 @@
       </c>
     </row>
     <row r="129">
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>waterfall</t>
+        </is>
+      </c>
       <c r="J129" t="inlineStr">
         <is>
           <t>used webjars.for</t>
@@ -3600,6 +3660,11 @@
       </c>
     </row>
     <row r="130">
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>agile/scrum</t>
+        </is>
+      </c>
       <c r="J130" t="inlineStr">
         <is>
           <t>client side libraries</t>
@@ -3607,6 +3672,11 @@
       </c>
     </row>
     <row r="131">
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>safe agile</t>
+        </is>
+      </c>
       <c r="J131" t="inlineStr">
         <is>
           <t>beans layers</t>
@@ -3614,6 +3684,11 @@
       </c>
     </row>
     <row r="132">
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>hld</t>
+        </is>
+      </c>
       <c r="J132" t="inlineStr">
         <is>
           <t>bean classes</t>
@@ -3621,6 +3696,11 @@
       </c>
     </row>
     <row r="133">
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>lld</t>
+        </is>
+      </c>
       <c r="J133" t="inlineStr">
         <is>
           <t>strong knowledge</t>
@@ -3628,6 +3708,11 @@
       </c>
     </row>
     <row r="134">
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>requirements definition</t>
+        </is>
+      </c>
       <c r="J134" t="inlineStr">
         <is>
           <t>test</t>
@@ -3635,6 +3720,11 @@
       </c>
     </row>
     <row r="135">
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>major systems</t>
+        </is>
+      </c>
       <c r="J135" t="inlineStr">
         <is>
           <t>certification</t>
@@ -3642,6 +3732,11 @@
       </c>
     </row>
     <row r="136">
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>user experience</t>
+        </is>
+      </c>
       <c r="J136" t="inlineStr">
         <is>
           <t>qspiders training</t>
@@ -3649,6 +3744,11 @@
       </c>
     </row>
     <row r="137">
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>ux</t>
+        </is>
+      </c>
       <c r="J137" t="inlineStr">
         <is>
           <t>technical skills</t>
@@ -3656,6 +3756,11 @@
       </c>
     </row>
     <row r="138">
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>user interactive</t>
+        </is>
+      </c>
       <c r="J138" t="inlineStr">
         <is>
           <t>strong</t>
@@ -3663,6 +3768,11 @@
       </c>
     </row>
     <row r="139">
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>ui</t>
+        </is>
+      </c>
       <c r="J139" t="inlineStr">
         <is>
           <t>software testing</t>
@@ -3670,6 +3780,11 @@
       </c>
     </row>
     <row r="140">
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>web pages jquery</t>
+        </is>
+      </c>
       <c r="J140" t="inlineStr">
         <is>
           <t>cycle</t>
@@ -3677,6 +3792,11 @@
       </c>
     </row>
     <row r="141">
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>redux</t>
+        </is>
+      </c>
       <c r="J141" t="inlineStr">
         <is>
           <t>smoke</t>
@@ -3684,6 +3804,11 @@
       </c>
     </row>
     <row r="142">
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>react-js</t>
+        </is>
+      </c>
       <c r="J142" t="inlineStr">
         <is>
           <t>basic knowledge</t>
@@ -3691,6 +3816,11 @@
       </c>
     </row>
     <row r="143">
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>expertise</t>
+        </is>
+      </c>
       <c r="J143" t="inlineStr">
         <is>
           <t>knowledge</t>
@@ -3698,6 +3828,11 @@
       </c>
     </row>
     <row r="144">
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>enterprise applications</t>
+        </is>
+      </c>
       <c r="J144" t="inlineStr">
         <is>
           <t>agile</t>
@@ -3705,6 +3840,11 @@
       </c>
     </row>
     <row r="145">
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>web</t>
+        </is>
+      </c>
       <c r="J145" t="inlineStr">
         <is>
           <t>severity</t>
@@ -3712,6 +3852,11 @@
       </c>
     </row>
     <row r="146">
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>web applications</t>
+        </is>
+      </c>
       <c r="J146" t="inlineStr">
         <is>
           <t>priority</t>
@@ -3719,6 +3864,11 @@
       </c>
     </row>
     <row r="147">
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>weblogic</t>
+        </is>
+      </c>
       <c r="J147" t="inlineStr">
         <is>
           <t>acceptance testing flexible</t>
@@ -3726,6 +3876,11 @@
       </c>
     </row>
     <row r="148">
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>websphere</t>
+        </is>
+      </c>
       <c r="J148" t="inlineStr">
         <is>
           <t>technical</t>
@@ -3733,6 +3888,11 @@
       </c>
     </row>
     <row r="149">
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>jboss application servers</t>
+        </is>
+      </c>
       <c r="J149" t="inlineStr">
         <is>
           <t>software</t>
@@ -3740,6 +3900,11 @@
       </c>
     </row>
     <row r="150">
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>tomcat</t>
+        </is>
+      </c>
       <c r="J150" t="inlineStr">
         <is>
           <t>development life</t>
@@ -3747,6 +3912,11 @@
       </c>
     </row>
     <row r="151">
+      <c r="I151" t="inlineStr">
+        <is>
+          <t>java ide</t>
+        </is>
+      </c>
       <c r="J151" t="inlineStr">
         <is>
           <t>build</t>
@@ -3754,6 +3924,11 @@
       </c>
     </row>
     <row r="152">
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>rational application developer</t>
+        </is>
+      </c>
       <c r="J152" t="inlineStr">
         <is>
           <t>release</t>
@@ -3761,6 +3936,11 @@
       </c>
     </row>
     <row r="153">
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>rad</t>
+        </is>
+      </c>
       <c r="J153" t="inlineStr">
         <is>
           <t>patch</t>
@@ -3768,6 +3948,11 @@
       </c>
     </row>
     <row r="154">
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>web sphere application developer</t>
+        </is>
+      </c>
       <c r="J154" t="inlineStr">
         <is>
           <t>test case</t>
@@ -3775,6 +3960,11 @@
       </c>
     </row>
     <row r="155">
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>wsad</t>
+        </is>
+      </c>
       <c r="J155" t="inlineStr">
         <is>
           <t>test scenario</t>
@@ -3782,6 +3972,11 @@
       </c>
     </row>
     <row r="156">
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>eclipse ee</t>
+        </is>
+      </c>
       <c r="J156" t="inlineStr">
         <is>
           <t>academic project details</t>
@@ -3789,6 +3984,11 @@
       </c>
     </row>
     <row r="157">
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>rsa</t>
+        </is>
+      </c>
       <c r="J157" t="inlineStr">
         <is>
           <t>course prediction using fidoop via online test</t>
@@ -3796,6 +3996,11 @@
       </c>
     </row>
     <row r="158">
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>netbeans</t>
+        </is>
+      </c>
       <c r="J158" t="inlineStr">
         <is>
           <t>primary extent</t>
@@ -3803,6 +4008,11 @@
       </c>
     </row>
     <row r="159">
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>dynamic web applications .. </t>
+        </is>
+      </c>
       <c r="J159" t="inlineStr">
         <is>
           <t>human knowledge</t>
@@ -3810,6 +4020,11 @@
       </c>
     </row>
     <row r="160">
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>hands-on</t>
+        </is>
+      </c>
       <c r="J160" t="inlineStr">
         <is>
           <t>strong points in myself</t>
@@ -3817,6 +4032,11 @@
       </c>
     </row>
     <row r="161">
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>source control tools</t>
+        </is>
+      </c>
       <c r="J161" t="inlineStr">
         <is>
           <t>social activities</t>
@@ -3824,6 +4044,11 @@
       </c>
     </row>
     <row r="162">
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>cvs</t>
+        </is>
+      </c>
       <c r="J162" t="inlineStr">
         <is>
           <t>grasping power</t>
@@ -3831,6 +4056,11 @@
       </c>
     </row>
     <row r="163">
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>clear case</t>
+        </is>
+      </c>
       <c r="J163" t="inlineStr">
         <is>
           <t>created</t>
@@ -3838,6 +4068,11 @@
       </c>
     </row>
     <row r="164">
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>svn</t>
+        </is>
+      </c>
       <c r="J164" t="inlineStr">
         <is>
           <t>gui</t>
@@ -3845,6 +4080,11 @@
       </c>
     </row>
     <row r="165">
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>git</t>
+        </is>
+      </c>
       <c r="J165" t="inlineStr">
         <is>
           <t>web pages</t>
@@ -3852,6 +4092,11 @@
       </c>
     </row>
     <row r="166">
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>surround scm</t>
+        </is>
+      </c>
       <c r="J166" t="inlineStr">
         <is>
           <t>jsp technical</t>
@@ -3859,6 +4104,11 @@
       </c>
     </row>
     <row r="167">
+      <c r="I167" t="inlineStr">
+        <is>
+          <t> work</t>
+        </is>
+      </c>
       <c r="J167" t="inlineStr">
         <is>
           <t>systems</t>
@@ -3866,6 +4116,11 @@
       </c>
     </row>
     <row r="168">
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>mockito</t>
+        </is>
+      </c>
       <c r="J168" t="inlineStr">
         <is>
           <t>windows-7</t>
@@ -3873,6 +4128,11 @@
       </c>
     </row>
     <row r="169">
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>firebug</t>
+        </is>
+      </c>
       <c r="J169" t="inlineStr">
         <is>
           <t>programming languages</t>
@@ -3880,6 +4140,11 @@
       </c>
     </row>
     <row r="170">
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>fireposter</t>
+        </is>
+      </c>
       <c r="J170" t="inlineStr">
         <is>
           <t>software</t>
@@ -3887,6 +4152,11 @@
       </c>
     </row>
     <row r="171">
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>soapui</t>
+        </is>
+      </c>
       <c r="J171" t="inlineStr">
         <is>
           <t>testing</t>
@@ -3894,6 +4164,11 @@
       </c>
     </row>
     <row r="172">
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>qa</t>
+        </is>
+      </c>
       <c r="J172" t="inlineStr">
         <is>
           <t>infotech</t>
@@ -3901,6 +4176,11 @@
       </c>
     </row>
     <row r="173">
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>good exposure</t>
+        </is>
+      </c>
       <c r="J173" t="inlineStr">
         <is>
           <t>challenging position</t>
@@ -3908,6 +4188,11 @@
       </c>
     </row>
     <row r="174">
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>application environment issues</t>
+        </is>
+      </c>
       <c r="J174" t="inlineStr">
         <is>
           <t>software engineer</t>
@@ -3915,6 +4200,11 @@
       </c>
     </row>
     <row r="175">
+      <c r="I175" t="inlineStr">
+        <is>
+          <t>different levels</t>
+        </is>
+      </c>
       <c r="J175" t="inlineStr">
         <is>
           <t>hardworking</t>
@@ -3922,6 +4212,11 @@
       </c>
     </row>
     <row r="176">
+      <c r="I176" t="inlineStr">
+        <is>
+          <t>internal teams</t>
+        </is>
+      </c>
       <c r="J176" t="inlineStr">
         <is>
           <t>quality services</t>
@@ -3929,6 +4224,11 @@
       </c>
     </row>
     <row r="177">
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>driven</t>
+        </is>
+      </c>
       <c r="J177" t="inlineStr">
         <is>
           <t>developing</t>
@@ -3936,6 +4236,11 @@
       </c>
     </row>
     <row r="178">
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>business environments</t>
+        </is>
+      </c>
       <c r="J178" t="inlineStr">
         <is>
           <t>code</t>
@@ -3943,6 +4248,11 @@
       </c>
     </row>
     <row r="179">
+      <c r="I179" t="inlineStr">
+        <is>
+          <t>experienced</t>
+        </is>
+      </c>
       <c r="J179" t="inlineStr">
         <is>
           <t>application systems</t>
@@ -3950,6 +4260,11 @@
       </c>
     </row>
     <row r="180">
+      <c r="I180" t="inlineStr">
+        <is>
+          <t>onsite</t>
+        </is>
+      </c>
       <c r="J180" t="inlineStr">
         <is>
           <t>designed</t>
@@ -3957,6 +4272,11 @@
       </c>
     </row>
     <row r="181">
+      <c r="I181" t="inlineStr">
+        <is>
+          <t>near</t>
+        </is>
+      </c>
       <c r="J181" t="inlineStr">
         <is>
           <t>various complex</t>
@@ -3964,6 +4284,11 @@
       </c>
     </row>
     <row r="182">
+      <c r="I182" t="inlineStr">
+        <is>
+          <t>offshore</t>
+        </is>
+      </c>
       <c r="J182" t="inlineStr">
         <is>
           <t>components jsp controller</t>
@@ -3971,6 +4296,11 @@
       </c>
     </row>
     <row r="183">
+      <c r="I183" t="inlineStr">
+        <is>
+          <t>pair programming</t>
+        </is>
+      </c>
       <c r="J183" t="inlineStr">
         <is>
           <t>hibernate configuration</t>
@@ -3978,6 +4308,11 @@
       </c>
     </row>
     <row r="184">
+      <c r="I184" t="inlineStr">
+        <is>
+          <t>ibm-clear case</t>
+        </is>
+      </c>
       <c r="J184" t="inlineStr">
         <is>
           <t>various modules</t>
@@ -3985,6 +4320,11 @@
       </c>
     </row>
     <row r="185">
+      <c r="I185" t="inlineStr">
+        <is>
+          <t>borland starteam designation software engineer</t>
+        </is>
+      </c>
       <c r="J185" t="inlineStr">
         <is>
           <t>client side validations</t>
@@ -3992,6 +4332,11 @@
       </c>
     </row>
     <row r="186">
+      <c r="I186" t="inlineStr">
+        <is>
+          <t>define billing plan/dates</t>
+        </is>
+      </c>
       <c r="J186" t="inlineStr">
         <is>
           <t>server</t>
@@ -3999,6 +4344,11 @@
       </c>
     </row>
     <row r="187">
+      <c r="I187" t="inlineStr">
+        <is>
+          <t>bill </t>
+        </is>
+      </c>
       <c r="J187" t="inlineStr">
         <is>
           <t>side validations</t>
@@ -4006,6 +4356,11 @@
       </c>
     </row>
     <row r="188">
+      <c r="I188" t="inlineStr">
+        <is>
+          <t>devops</t>
+        </is>
+      </c>
       <c r="J188" t="inlineStr">
         <is>
           <t>written jsp</t>
@@ -4013,6 +4368,11 @@
       </c>
     </row>
     <row r="189">
+      <c r="I189" t="inlineStr">
+        <is>
+          <t>user interfaces</t>
+        </is>
+      </c>
       <c r="J189" t="inlineStr">
         <is>
           <t></t>
@@ -4020,6 +4380,11 @@
       </c>
     </row>
     <row r="190">
+      <c r="I190" t="inlineStr">
+        <is>
+          <t>css3</t>
+        </is>
+      </c>
       <c r="J190" t="inlineStr">
         <is>
           <t></t>
@@ -4027,6 +4392,11 @@
       </c>
     </row>
     <row r="191">
+      <c r="I191" t="inlineStr">
+        <is>
+          <t>sass</t>
+        </is>
+      </c>
       <c r="J191" t="inlineStr">
         <is>
           <t></t>
@@ -4034,6 +4404,11 @@
       </c>
     </row>
     <row r="192">
+      <c r="I192" t="inlineStr">
+        <is>
+          <t>skills profile java j2ee</t>
+        </is>
+      </c>
       <c r="J192" t="inlineStr">
         <is>
           <t>aop</t>
@@ -4041,6 +4416,11 @@
       </c>
     </row>
     <row r="193">
+      <c r="I193" t="inlineStr">
+        <is>
+          <t>jpa</t>
+        </is>
+      </c>
       <c r="J193" t="inlineStr">
         <is>
           <t>mvc</t>
@@ -4048,6 +4428,11 @@
       </c>
     </row>
     <row r="194">
+      <c r="I194" t="inlineStr">
+        <is>
+          <t>jax-rpc/ws/rs</t>
+        </is>
+      </c>
       <c r="J194" t="inlineStr">
         <is>
           <t>orm</t>
@@ -4055,6 +4440,11 @@
       </c>
     </row>
     <row r="195">
+      <c r="I195" t="inlineStr">
+        <is>
+          <t>jaxb</t>
+        </is>
+      </c>
       <c r="J195" t="inlineStr">
         <is>
           <t>sql developer</t>
@@ -4062,6 +4452,11 @@
       </c>
     </row>
     <row r="196">
+      <c r="I196" t="inlineStr">
+        <is>
+          <t>pl/sql docker</t>
+        </is>
+      </c>
       <c r="J196" t="inlineStr">
         <is>
           <t></t>
@@ -4069,6 +4464,11 @@
       </c>
     </row>
     <row r="197">
+      <c r="I197" t="inlineStr">
+        <is>
+          <t>jenkins</t>
+        </is>
+      </c>
       <c r="J197" t="inlineStr">
         <is>
           <t>frameworks certification</t>
@@ -4076,278 +4476,2593 @@
       </c>
     </row>
     <row r="198">
+      <c r="I198" t="inlineStr">
+        <is>
+          <t>dyna trace</t>
+        </is>
+      </c>
       <c r="J198" t="inlineStr">
         <is>
           <t>performing</t>
         </is>
       </c>
     </row>
-    <row r="199"/>
-    <row r="200"/>
-    <row r="201"/>
-    <row r="202"/>
-    <row r="203"/>
-    <row r="204"/>
-    <row r="205"/>
-    <row r="206"/>
-    <row r="207"/>
-    <row r="208"/>
-    <row r="209"/>
-    <row r="210"/>
-    <row r="211"/>
-    <row r="212"/>
-    <row r="213"/>
-    <row r="214"/>
-    <row r="215"/>
-    <row r="216"/>
-    <row r="217"/>
-    <row r="218"/>
-    <row r="219"/>
-    <row r="220"/>
-    <row r="221"/>
-    <row r="222"/>
-    <row r="223"/>
-    <row r="224"/>
-    <row r="225"/>
-    <row r="226"/>
-    <row r="227"/>
-    <row r="228"/>
-    <row r="229"/>
-    <row r="230"/>
-    <row r="231"/>
-    <row r="232"/>
-    <row r="233"/>
-    <row r="234"/>
-    <row r="235"/>
-    <row r="236"/>
-    <row r="237"/>
-    <row r="238"/>
-    <row r="239"/>
-    <row r="240"/>
-    <row r="241"/>
-    <row r="242"/>
-    <row r="243"/>
-    <row r="244"/>
-    <row r="245"/>
-    <row r="246"/>
-    <row r="247"/>
-    <row r="248"/>
-    <row r="249"/>
-    <row r="250"/>
-    <row r="251"/>
-    <row r="252"/>
-    <row r="253"/>
-    <row r="254"/>
-    <row r="255"/>
-    <row r="256"/>
-    <row r="257"/>
-    <row r="258"/>
-    <row r="259"/>
-    <row r="260"/>
-    <row r="261"/>
-    <row r="262"/>
-    <row r="263"/>
-    <row r="264"/>
-    <row r="265"/>
-    <row r="266"/>
-    <row r="267"/>
-    <row r="268"/>
-    <row r="269"/>
-    <row r="270"/>
-    <row r="271"/>
-    <row r="272"/>
-    <row r="273"/>
-    <row r="274"/>
-    <row r="275"/>
-    <row r="276"/>
-    <row r="277"/>
-    <row r="278"/>
-    <row r="279"/>
-    <row r="280"/>
-    <row r="281"/>
-    <row r="282"/>
-    <row r="283"/>
-    <row r="284"/>
-    <row r="285"/>
-    <row r="286"/>
-    <row r="287"/>
-    <row r="288"/>
-    <row r="289"/>
-    <row r="290"/>
-    <row r="291"/>
-    <row r="292"/>
-    <row r="293"/>
-    <row r="294"/>
-    <row r="295"/>
-    <row r="296"/>
-    <row r="297"/>
-    <row r="298"/>
-    <row r="299"/>
-    <row r="300"/>
-    <row r="301"/>
-    <row r="302"/>
-    <row r="303"/>
-    <row r="304"/>
-    <row r="305"/>
-    <row r="306"/>
-    <row r="307"/>
-    <row r="308"/>
-    <row r="309"/>
-    <row r="310"/>
-    <row r="311"/>
-    <row r="312"/>
-    <row r="313"/>
-    <row r="314"/>
-    <row r="315"/>
-    <row r="316"/>
-    <row r="317"/>
-    <row r="318"/>
-    <row r="319"/>
-    <row r="320"/>
-    <row r="321"/>
-    <row r="322"/>
-    <row r="323"/>
-    <row r="324"/>
-    <row r="325"/>
-    <row r="326"/>
-    <row r="327"/>
-    <row r="328"/>
-    <row r="329"/>
-    <row r="330"/>
-    <row r="331"/>
-    <row r="332"/>
-    <row r="333"/>
-    <row r="334"/>
-    <row r="335"/>
-    <row r="336"/>
-    <row r="337"/>
-    <row r="338"/>
-    <row r="339"/>
-    <row r="340"/>
-    <row r="341"/>
-    <row r="342"/>
-    <row r="343"/>
-    <row r="344"/>
-    <row r="345"/>
-    <row r="346"/>
-    <row r="347"/>
-    <row r="348"/>
-    <row r="349"/>
-    <row r="350"/>
-    <row r="351"/>
-    <row r="352"/>
-    <row r="353"/>
-    <row r="354"/>
-    <row r="355"/>
-    <row r="356"/>
-    <row r="357"/>
-    <row r="358"/>
-    <row r="359"/>
-    <row r="360"/>
-    <row r="361"/>
-    <row r="362"/>
-    <row r="363"/>
-    <row r="364"/>
-    <row r="365"/>
-    <row r="366"/>
-    <row r="367"/>
-    <row r="368"/>
-    <row r="369"/>
-    <row r="370"/>
-    <row r="371"/>
-    <row r="372"/>
-    <row r="373"/>
-    <row r="374"/>
-    <row r="375"/>
-    <row r="376"/>
-    <row r="377"/>
-    <row r="378"/>
-    <row r="379"/>
-    <row r="380"/>
-    <row r="381"/>
-    <row r="382"/>
-    <row r="383"/>
-    <row r="384"/>
-    <row r="385"/>
-    <row r="386"/>
-    <row r="387"/>
-    <row r="388"/>
-    <row r="389"/>
-    <row r="390"/>
-    <row r="391"/>
-    <row r="392"/>
-    <row r="393"/>
-    <row r="394"/>
-    <row r="395"/>
-    <row r="396"/>
-    <row r="397"/>
-    <row r="398"/>
-    <row r="399"/>
-    <row r="400"/>
-    <row r="401"/>
-    <row r="402"/>
-    <row r="403"/>
-    <row r="404"/>
-    <row r="405"/>
-    <row r="406"/>
-    <row r="407"/>
-    <row r="408"/>
-    <row r="409"/>
-    <row r="410"/>
-    <row r="411"/>
-    <row r="412"/>
-    <row r="413"/>
-    <row r="414"/>
-    <row r="415"/>
-    <row r="416"/>
-    <row r="417"/>
-    <row r="418"/>
-    <row r="419"/>
-    <row r="420"/>
-    <row r="421"/>
-    <row r="422"/>
-    <row r="423"/>
-    <row r="424"/>
-    <row r="425"/>
-    <row r="426"/>
-    <row r="427"/>
-    <row r="428"/>
-    <row r="429"/>
-    <row r="430"/>
-    <row r="431"/>
-    <row r="432"/>
-    <row r="433"/>
-    <row r="434"/>
-    <row r="435"/>
-    <row r="436"/>
-    <row r="437"/>
-    <row r="438"/>
-    <row r="439"/>
-    <row r="440"/>
-    <row r="441"/>
-    <row r="442"/>
-    <row r="443"/>
-    <row r="444"/>
-    <row r="445"/>
-    <row r="446"/>
-    <row r="447"/>
-    <row r="448"/>
-    <row r="449"/>
-    <row r="450"/>
-    <row r="451"/>
-    <row r="452"/>
-    <row r="453"/>
-    <row r="454"/>
-    <row r="455"/>
-    <row r="456"/>
-    <row r="457"/>
-    <row r="458"/>
-    <row r="459"/>
-    <row r="460"/>
-    <row r="461"/>
-    <row r="462"/>
-    <row r="463"/>
-    <row r="464"/>
+    <row r="199">
+      <c r="I199" t="inlineStr">
+        <is>
+          <t>gradle</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="I200" t="inlineStr">
+        <is>
+          <t>ready api</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="I201" t="inlineStr">
+        <is>
+          <t>kubernetes</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="I202" t="inlineStr">
+        <is>
+          <t>grafana</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="I203" t="inlineStr">
+        <is>
+          <t>kibana</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="I204" t="inlineStr">
+        <is>
+          <t>prometheus micro</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="I205" t="inlineStr">
+        <is>
+          <t>jms json</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="I206" t="inlineStr">
+        <is>
+          <t>xsd</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="I207" t="inlineStr">
+        <is>
+          <t>hibernate</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="I208" t="inlineStr">
+        <is>
+          <t>struts</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="I209" t="inlineStr">
+        <is>
+          <t>wicket</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="I210" t="inlineStr">
+        <is>
+          <t>internet portal framework</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="I211" t="inlineStr">
+        <is>
+          <t>ipf</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="I212" t="inlineStr">
+        <is>
+          <t>presentation</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="I213" t="inlineStr">
+        <is>
+          <t>framework html</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="I214" t="inlineStr">
+        <is>
+          <t>es6</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="I215" t="inlineStr">
+        <is>
+          <t>react</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="I216" t="inlineStr">
+        <is>
+          <t>node js</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="I217" t="inlineStr">
+        <is>
+          <t>db2</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="I218" t="inlineStr">
+        <is>
+          <t>oracle</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="I219" t="inlineStr">
+        <is>
+          <t>udb</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="I220" t="inlineStr">
+        <is>
+          <t>mysql testing frameworks application servers ibm-websphere</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="I221" t="inlineStr">
+        <is>
+          <t>apache tomcat</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="I222" t="inlineStr">
+        <is>
+          <t>jboss ibm-rsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="I223" t="inlineStr">
+        <is>
+          <t>eclipse</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="I224" t="inlineStr">
+        <is>
+          <t>vscode</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="I225" t="inlineStr">
+        <is>
+          <t>visio</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="I226" t="inlineStr">
+        <is>
+          <t>putty</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="I227" t="inlineStr">
+        <is>
+          <t>sql squirrel</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="I228" t="inlineStr">
+        <is>
+          <t>webstorm</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="I229" t="inlineStr">
+        <is>
+          <t>sql ibm-clear quest</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="I230" t="inlineStr">
+        <is>
+          <t>rtc</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="I231" t="inlineStr">
+        <is>
+          <t>jira agile/scrum</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="I232" t="inlineStr">
+        <is>
+          <t>lean</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="I233" t="inlineStr">
+        <is>
+          <t>iterative</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="I234" t="inlineStr">
+        <is>
+          <t>lab agile</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="I235" t="inlineStr">
+        <is>
+          <t> design</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="I236" t="inlineStr">
+        <is>
+          <t>rest apis</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="I237" t="inlineStr">
+        <is>
+          <t>restfull api</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="I238" t="inlineStr">
+        <is>
+          <t>conducted</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="I239" t="inlineStr">
+        <is>
+          <t>entire portfolio</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="I240" t="inlineStr">
+        <is>
+          <t>200+ associates</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="I241" t="inlineStr">
+        <is>
+          <t>period</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="I242" t="inlineStr">
+        <is>
+          <t>dec</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="I243" t="inlineStr">
+        <is>
+          <t>software engineering lead</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="I244" t="inlineStr">
+        <is>
+          <t>senior management</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="I245" t="inlineStr">
+        <is>
+          <t>data formats junit</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="I246" t="inlineStr">
+        <is>
+          <t>power mockito</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="I247" t="inlineStr">
+        <is>
+          <t>mocha</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="I248" t="inlineStr">
+        <is>
+          <t>chai</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="I249" t="inlineStr">
+        <is>
+          <t>developer</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="I250" t="inlineStr">
+        <is>
+          <t>ant</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="I251" t="inlineStr">
+        <is>
+          <t>intellij project methodologies tata consultancy</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="I252" t="inlineStr">
+        <is>
+          <t>associate consultant project title</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="I253" t="inlineStr">
+        <is>
+          <t>billing transformation</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="I254" t="inlineStr">
+        <is>
+          <t>august</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="I255" t="inlineStr">
+        <is>
+          <t>automobile</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="I256" t="inlineStr">
+        <is>
+          <t>usaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="I257" t="inlineStr">
+        <is>
+          <t>enterprise billing system</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="I258" t="inlineStr">
+        <is>
+          <t>business ’ s whenever</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="I259" t="inlineStr">
+        <is>
+          <t>product</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="I260" t="inlineStr">
+        <is>
+          <t>billing system</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="I261" t="inlineStr">
+        <is>
+          <t>integration opportunities</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="I262" t="inlineStr">
+        <is>
+          <t>billing capabilities</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="I263" t="inlineStr">
+        <is>
+          <t>enterprise money movement payment capabilities</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="I264" t="inlineStr">
+        <is>
+          <t>real time</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="I265" t="inlineStr">
+        <is>
+          <t>executing</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="I266" t="inlineStr">
+        <is>
+          <t>cas payment</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="I267" t="inlineStr">
+        <is>
+          <t>billing</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="I268" t="inlineStr">
+        <is>
+          <t>enterprise money movement system</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="I269" t="inlineStr">
+        <is>
+          <t>enterprise billing capabilities</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="I270" t="inlineStr">
+        <is>
+          <t>reduce complexity</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="I271" t="inlineStr">
+        <is>
+          <t>business users e. post</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="I272" t="inlineStr">
+        <is>
+          <t>overpayment</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="I273" t="inlineStr">
+        <is>
+          <t>underpayment</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="I274" t="inlineStr">
+        <is>
+          <t>due amount f.</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="I275" t="inlineStr">
+        <is>
+          <t>mortgagee</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="I276" t="inlineStr">
+        <is>
+          <t>received</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="I277" t="inlineStr">
+        <is>
+          <t>splunk</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="I278" t="inlineStr">
+        <is>
+          <t>developed</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="I279" t="inlineStr">
+        <is>
+          <t>test data preparation tool</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="I280" t="inlineStr">
+        <is>
+          <t>% time</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="I281" t="inlineStr">
+        <is>
+          <t>came</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="I282" t="inlineStr">
+        <is>
+          <t>high available test environment</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="I283" t="inlineStr">
+        <is>
+          <t>support </t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="I284" t="inlineStr">
+        <is>
+          <t>established</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="I285" t="inlineStr">
+        <is>
+          <t>environment support team</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="I286" t="inlineStr">
+        <is>
+          <t>systems team</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="I287" t="inlineStr">
+        <is>
+          <t>quality assurance team scrum</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="I288" t="inlineStr">
+        <is>
+          <t>safe</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="I289" t="inlineStr">
+        <is>
+          <t>project title</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="I290" t="inlineStr">
+        <is>
+          <t>digital parity</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="I291" t="inlineStr">
+        <is>
+          <t>– money</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="I292" t="inlineStr">
+        <is>
+          <t>movement period</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="I293" t="inlineStr">
+        <is>
+          <t>feb</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="I294" t="inlineStr">
+        <is>
+          <t>july</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="I295" t="inlineStr">
+        <is>
+          <t>accelerate</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="I296" t="inlineStr">
+        <is>
+          <t>movement</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="I297" t="inlineStr">
+        <is>
+          <t>member satisfaction</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="I298" t="inlineStr">
+        <is>
+          <t>contact center</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="I299" t="inlineStr">
+        <is>
+          <t>self-service capabilities</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="I300" t="inlineStr">
+        <is>
+          <t>provide</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="I301" t="inlineStr">
+        <is>
+          <t>iphone app</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="I302" t="inlineStr">
+        <is>
+          <t>android</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="I303" t="inlineStr">
+        <is>
+          <t>ipad</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="I304" t="inlineStr">
+        <is>
+          <t>mobile web site</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="I305" t="inlineStr">
+        <is>
+          <t>setup</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="I306" t="inlineStr">
+        <is>
+          <t>automatic payment plan</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="I307" t="inlineStr">
+        <is>
+          <t>internal bills</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="I308" t="inlineStr">
+        <is>
+          <t>accomplishments</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="I309" t="inlineStr">
+        <is>
+          <t>ibm</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="I310" t="inlineStr">
+        <is>
+          <t>junit code coverage</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="I311" t="inlineStr">
+        <is>
+          <t>provided</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="I312" t="inlineStr">
+        <is>
+          <t>standard </t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="I313" t="inlineStr">
+        <is>
+          <t>new age technologies</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="I314" t="inlineStr">
+        <is>
+          <t>knowledge delivery period</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="I315" t="inlineStr">
+        <is>
+          <t>april</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="I316" t="inlineStr">
+        <is>
+          <t>jan</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="I317" t="inlineStr">
+        <is>
+          <t>lead</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="I318" t="inlineStr">
+        <is>
+          <t>empower member</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="I319" t="inlineStr">
+        <is>
+          <t>msrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="I320" t="inlineStr">
+        <is>
+          <t>right time</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="I321" t="inlineStr">
+        <is>
+          <t>consistent experiences</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="I322" t="inlineStr">
+        <is>
+          <t>reduce msr</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="I323" t="inlineStr">
+        <is>
+          <t>member experience</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="I324" t="inlineStr">
+        <is>
+          <t>continue</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="I325" t="inlineStr">
+        <is>
+          <t>knowledge delivery</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="I326" t="inlineStr">
+        <is>
+          <t>bank products</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="I327" t="inlineStr">
+        <is>
+          <t>deposits</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="I328" t="inlineStr">
+        <is>
+          <t>credit</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="I329" t="inlineStr">
+        <is>
+          <t>equity</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="I330" t="inlineStr">
+        <is>
+          <t>originations accomplishments</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="I331" t="inlineStr">
+        <is>
+          <t>learned xslt</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="I332" t="inlineStr">
+        <is>
+          <t>migrate html content</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="I333" t="inlineStr">
+        <is>
+          <t>customer accolades</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="I334" t="inlineStr">
+        <is>
+          <t>sprint</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="I335" t="inlineStr">
+        <is>
+          <t>showcase offshore team capability</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="I336" t="inlineStr">
+        <is>
+          <t>modular eligibility</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="I337" t="inlineStr">
+        <is>
+          <t>personal</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="I338" t="inlineStr">
+        <is>
+          <t>sep</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="I339" t="inlineStr">
+        <is>
+          <t>march</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="I340" t="inlineStr">
+        <is>
+          <t>project lead create</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="I341" t="inlineStr">
+        <is>
+          <t>reusable application</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="I342" t="inlineStr">
+        <is>
+          <t>eligibility information</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="I343" t="inlineStr">
+        <is>
+          <t>personal information rules</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="I344" t="inlineStr">
+        <is>
+          <t>widgets</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="I345" t="inlineStr">
+        <is>
+          <t>product application requirements</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="I346" t="inlineStr">
+        <is>
+          <t>establish</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="I347" t="inlineStr">
+        <is>
+          <t>probable members</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="I348" t="inlineStr">
+        <is>
+          <t>implement</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="I349" t="inlineStr">
+        <is>
+          <t>service side applications</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="I350" t="inlineStr">
+        <is>
+          <t>pre-fill</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="I351" t="inlineStr">
+        <is>
+          <t>personal information application</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="I352" t="inlineStr">
+        <is>
+          <t>personalize content</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="I353" t="inlineStr">
+        <is>
+          <t>incorporate</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="I354" t="inlineStr">
+        <is>
+          <t>reusable personal information widget</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="I355" t="inlineStr">
+        <is>
+          <t>conducted kt</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="I356" t="inlineStr">
+        <is>
+          <t>new joiners</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="I357" t="inlineStr">
+        <is>
+          <t>development environment</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="I358" t="inlineStr">
+        <is>
+          <t>project name</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="I359" t="inlineStr">
+        <is>
+          <t>prospect registration period</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="I360" t="inlineStr">
+        <is>
+          <t>oct</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="I361" t="inlineStr">
+        <is>
+          <t>aug</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="I362" t="inlineStr">
+        <is>
+          <t>module lead creating</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="I363" t="inlineStr">
+        <is>
+          <t>prospects</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="I364" t="inlineStr">
+        <is>
+          <t>saved</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="I365" t="inlineStr">
+        <is>
+          <t>quotes</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="I366" t="inlineStr">
+        <is>
+          <t>calculators</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="I367" t="inlineStr">
+        <is>
+          <t>easy transition</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="I368" t="inlineStr">
+        <is>
+          <t>project modifies</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="I369" t="inlineStr">
+        <is>
+          <t>member eligibility application</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="I370" t="inlineStr">
+        <is>
+          <t>member</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="I371" t="inlineStr">
+        <is>
+          <t>migration</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="I372" t="inlineStr">
+        <is>
+          <t>star team</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="I373" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="I374" t="inlineStr">
+        <is>
+          <t>scrum team</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="I375" t="inlineStr">
+        <is>
+          <t>developer / tester</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="I376" t="inlineStr">
+        <is>
+          <t>bd</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="I377" t="inlineStr">
+        <is>
+          <t>leads repository period</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="I378" t="inlineStr">
+        <is>
+          <t>module lead implement</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="I379" t="inlineStr">
+        <is>
+          <t>salesforce.com software solution</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="I380" t="inlineStr">
+        <is>
+          <t>member delivery</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="I381" t="inlineStr">
+        <is>
+          <t>partnership</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="I382" t="inlineStr">
+        <is>
+          <t>gathering non member sales</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="I383" t="inlineStr">
+        <is>
+          <t>integrated salesforce.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="I384" t="inlineStr">
+        <is>
+          <t>communicate</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="I385" t="inlineStr">
+        <is>
+          <t>generate</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="I386" t="inlineStr">
+        <is>
+          <t>follow-up communications</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="I387" t="inlineStr">
+        <is>
+          <t>multi-wave contacts</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="I388" t="inlineStr">
+        <is>
+          <t>support</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="I389" t="inlineStr">
+        <is>
+          <t>multiple prospect lead type</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="I390" t="inlineStr">
+        <is>
+          <t>determine</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="I391" t="inlineStr">
+        <is>
+          <t>campaign type</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="I392" t="inlineStr">
+        <is>
+          <t>exclude</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="I393" t="inlineStr">
+        <is>
+          <t>exclusion rules</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="I394" t="inlineStr">
+        <is>
+          <t>new prospects</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="I395" t="inlineStr">
+        <is>
+          <t>salesforce</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="I396" t="inlineStr">
+        <is>
+          <t>co-ordination</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="I397" t="inlineStr">
+        <is>
+          <t>quality assurance team</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="I398" t="inlineStr">
+        <is>
+          <t>annuity</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="I399" t="inlineStr">
+        <is>
+          <t>reporting period</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="I400" t="inlineStr">
+        <is>
+          <t>senior developer</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="I401" t="inlineStr">
+        <is>
+          <t>life insurance company</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="I402" t="inlineStr">
+        <is>
+          <t>direct response company</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="I403" t="inlineStr">
+        <is>
+          <t>necessary information</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="I404" t="inlineStr">
+        <is>
+          <t>replacement contracts</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="I405" t="inlineStr">
+        <is>
+          <t>acquisition flow</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="I406" t="inlineStr">
+        <is>
+          <t>modify</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="I407" t="inlineStr">
+        <is>
+          <t>annuity acquisition processes</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="I408" t="inlineStr">
+        <is>
+          <t>usaa.com/portal</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="I409" t="inlineStr">
+        <is>
+          <t>screens</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="I410" t="inlineStr">
+        <is>
+          <t>agency requirements</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="I411" t="inlineStr">
+        <is>
+          <t>collect</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="I412" t="inlineStr">
+        <is>
+          <t>member ’ s responses</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="I413" t="inlineStr">
+        <is>
+          <t>replacement questions</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="I414" t="inlineStr">
+        <is>
+          <t>populate responses</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="I415" t="inlineStr">
+        <is>
+          <t>replacement form</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="I416" t="inlineStr">
+        <is>
+          <t>ability</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="I417" t="inlineStr">
+        <is>
+          <t>agency replacement requirements</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="I418" t="inlineStr">
+        <is>
+          <t>green screens</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="I419" t="inlineStr">
+        <is>
+          <t>zero defects</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="I420" t="inlineStr">
+        <is>
+          <t>roaap dual</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="I421" t="inlineStr">
+        <is>
+          <t>fulfillment systems</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="I422" t="inlineStr">
+        <is>
+          <t>msa</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="I423" t="inlineStr">
+        <is>
+          <t>initiate</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="I424" t="inlineStr">
+        <is>
+          <t>annuity acquisition toll</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="I425" t="inlineStr">
+        <is>
+          <t>support compliance</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="I426" t="inlineStr">
+        <is>
+          <t>annuity acquisition</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="I427" t="inlineStr">
+        <is>
+          <t>update</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="I428" t="inlineStr">
+        <is>
+          <t>fulfilment systems</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="I429" t="inlineStr">
+        <is>
+          <t>roaap</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="I430" t="inlineStr">
+        <is>
+          <t>income annuity acquisition flow</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="I431" t="inlineStr">
+        <is>
+          <t>turn</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="I432" t="inlineStr">
+        <is>
+          <t>shadow</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="I433" t="inlineStr">
+        <is>
+          <t>keep msa</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="I434" t="inlineStr">
+        <is>
+          <t>msa roaap</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="I435" t="inlineStr">
+        <is>
+          <t>updating</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="I436" t="inlineStr">
+        <is>
+          <t>iop</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="I437" t="inlineStr">
+        <is>
+          <t>liis</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="I438" t="inlineStr">
+        <is>
+          <t>fps</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="I439" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="I440" t="inlineStr">
+        <is>
+          <t>annuities areas</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="I441" t="inlineStr">
+        <is>
+          <t>role bases authentication</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="I442" t="inlineStr">
+        <is>
+          <t>content generation</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="I443" t="inlineStr">
+        <is>
+          <t>web content</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="I444" t="inlineStr">
+        <is>
+          <t>configuration team</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="I445" t="inlineStr">
+        <is>
+          <t>account verification client</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="I446" t="inlineStr">
+        <is>
+          <t>validate</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="I447" t="inlineStr">
+        <is>
+          <t>financial institution account</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="I448" t="inlineStr">
+        <is>
+          <t>external account database</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="I449" t="inlineStr">
+        <is>
+          <t>deposit fraud losses</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="I450" t="inlineStr">
+        <is>
+          <t>account</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="I451" t="inlineStr">
+        <is>
+          <t>manage accounts</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="I452" t="inlineStr">
+        <is>
+          <t>instant verification</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="I453" t="inlineStr">
+        <is>
+          <t>trial-deposit verification services</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="I454" t="inlineStr">
+        <is>
+          <t>cashedge</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="I455" t="inlineStr">
+        <is>
+          <t>inc</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="I456" t="inlineStr">
+        <is>
+          <t>convert</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="I457" t="inlineStr">
+        <is>
+          <t>manage accounts msr portal</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="I458" t="inlineStr">
+        <is>
+          <t>proposed</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="I459" t="inlineStr">
+        <is>
+          <t>externalization business rules</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="I460" t="inlineStr">
+        <is>
+          <t>ilog jrules</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="I461" t="inlineStr">
+        <is>
+          <t>configuration management team</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="I462" t="inlineStr">
+        <is>
+          <t>support web sphere application server</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="I463" t="inlineStr">
+        <is>
+          <t>development team</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="I464" t="inlineStr">
+        <is>
+          <t>designing</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="I465" t="inlineStr">
+        <is>
+          <t>user interface</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="I466" t="inlineStr">
+        <is>
+          <t>web application</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="I467" t="inlineStr">
+        <is>
+          <t>html5</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="I468" t="inlineStr">
+        <is>
+          <t>angular8</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="I469" t="inlineStr">
+        <is>
+          <t>css3</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="I470" t="inlineStr">
+        <is>
+          <t>pipe</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="I471" t="inlineStr">
+        <is>
+          <t>computer</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="I472" t="inlineStr">
+        <is>
+          <t>c++</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="I473" t="inlineStr">
+        <is>
+          <t>attended</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="I474" t="inlineStr">
+        <is>
+          <t>certification course</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="I475" t="inlineStr">
+        <is>
+          <t>credo systemz</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="I476" t="inlineStr">
+        <is>
+          <t>velachery</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="I477" t="inlineStr">
+        <is>
+          <t>b.tech title</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="I478" t="inlineStr">
+        <is>
+          <t>key</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="I479" t="inlineStr">
+        <is>
+          <t>aggregate cryptosystem</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="I480" t="inlineStr">
+        <is>
+          <t>scalable data</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="I481" t="inlineStr">
+        <is>
+          <t>cloud storage</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="I482" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="I483" t="inlineStr">
+        <is>
+          <t>cloud computing title</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="I484" t="inlineStr">
+        <is>
+          <t>perceive fraudulent recommenders</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="I485" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="I486" t="inlineStr">
+        <is>
+          <t>networks domain</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="I487" t="inlineStr">
+        <is>
+          <t>network</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="I488" t="inlineStr">
+        <is>
+          <t>dishonest users</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="I489" t="inlineStr">
+        <is>
+          <t>companies opinion</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="I490" t="inlineStr">
+        <is>
+          <t>e-commerce application created</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="I491" t="inlineStr">
+        <is>
+          <t>components</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="I492" t="inlineStr">
+        <is>
+          <t>directives</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="I493" t="inlineStr">
+        <is>
+          <t>pipes/filters</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="I494" t="inlineStr">
+        <is>
+          <t>created routing</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="I495" t="inlineStr">
+        <is>
+          <t>angular router</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="I496" t="inlineStr">
+        <is>
+          <t>custom attribute directives</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="I497" t="inlineStr">
+        <is>
+          <t>input validations</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="I498" t="inlineStr">
+        <is>
+          <t>web</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="I499" t="inlineStr">
+        <is>
+          <t>capability</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="I500" t="inlineStr">
+        <is>
+          <t>career objective an overview excellent communication</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="I501" t="inlineStr">
+        <is>
+          <t>interpersonal skills</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="I502" t="inlineStr">
+        <is>
+          <t>will</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="I503" t="inlineStr">
+        <is>
+          <t>urge</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="I504" t="inlineStr">
+        <is>
+          <t>technologies</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="I505" t="inlineStr">
+        <is>
+          <t>attended</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="I506" t="inlineStr">
+        <is>
+          <t>certification course</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="I507" t="inlineStr">
+        <is>
+          <t>javascript and angular</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="I508" t="inlineStr">
+        <is>
+          <t>credo systemz</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="I509" t="inlineStr">
+        <is>
+          <t>velachery designing</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="I510" t="inlineStr">
+        <is>
+          <t>user interface</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="I511" t="inlineStr">
+        <is>
+          <t>web application</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="I512" t="inlineStr">
+        <is>
+          <t>html5</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="I513" t="inlineStr">
+        <is>
+          <t>angularjs</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="I514" t="inlineStr">
+        <is>
+          <t>css3</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="I515" t="inlineStr">
+        <is>
+          <t>pipe</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="I516" t="inlineStr">
+        <is>
+          <t>proficient</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="I517" t="inlineStr">
+        <is>
+          <t>adept</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="I518" t="inlineStr">
+        <is>
+          <t>requirements</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="I519" t="inlineStr">
+        <is>
+          <t>complex application problems</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="I520" t="inlineStr">
+        <is>
+          <t>academic projects e-commerce application created</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="I521" t="inlineStr">
+        <is>
+          <t>components</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="I522" t="inlineStr">
+        <is>
+          <t>directives</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="I523" t="inlineStr">
+        <is>
+          <t>pipes/filters</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="I524" t="inlineStr">
+        <is>
+          <t>created routing</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="I525" t="inlineStr">
+        <is>
+          <t>angular router</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="I526" t="inlineStr">
+        <is>
+          <t>custom attribute directives</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="I527" t="inlineStr">
+        <is>
+          <t>input validations</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="I528" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="I529" t="inlineStr">
+        <is>
+          <t>maintaining lifetime</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="I530" t="inlineStr">
+        <is>
+          <t>wireless adhoc sensor networks</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="I531" t="inlineStr">
+        <is>
+          <t>mitigating vampire</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="I532" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="I533" t="inlineStr">
+        <is>
+          <t>wireless sensor networks</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="I534" t="inlineStr">
+        <is>
+          <t>vampire attacks</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="I535" t="inlineStr">
+        <is>
+          <t>tech title</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="I536" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="I537" t="inlineStr">
+        <is>
+          <t>query dependent ranking</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="I538" t="inlineStr">
+        <is>
+          <t>web databases related</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="I539" t="inlineStr">
+        <is>
+          <t>automobile sector domain</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="I540" t="inlineStr">
+        <is>
+          <t>data mining</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="I541" t="inlineStr">
+        <is>
+          <t>query results</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="I542" t="inlineStr">
+        <is>
+          <t>web databases</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="I543" t="inlineStr">
+        <is>
+          <t>dependent models</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="I544" t="inlineStr">
+        <is>
+          <t>career objective</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="I545" t="inlineStr">
+        <is>
+          <t>healthy work environment</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="I546" t="inlineStr">
+        <is>
+          <t>organizational growth</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="I547" t="inlineStr">
+        <is>
+          <t>skills known</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="I548" t="inlineStr">
+        <is>
+          <t>scripting language</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="I549" t="inlineStr">
+        <is>
+          <t>type script</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="I550" t="inlineStr">
+        <is>
+          <t>nodejs</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="I551" t="inlineStr">
+        <is>
+          <t>scripting framework</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="I552" t="inlineStr">
+        <is>
+          <t>windows versions/linux</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="I553" t="inlineStr">
+        <is>
+          <t>angular7</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="I554" t="inlineStr">
+        <is>
+          <t>ionic/cordova</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="I555" t="inlineStr">
+        <is>
+          <t>interest</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="I556" t="inlineStr">
+        <is>
+          <t>willing</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="I557" t="inlineStr">
+        <is>
+          <t>web</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="I558" t="inlineStr">
+        <is>
+          <t>app development</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="I559" t="inlineStr">
+        <is>
+          <t>participated</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="I560" t="inlineStr">
+        <is>
+          <t>ethical hacking</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="I561" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="I562" t="inlineStr">
+        <is>
+          <t>r.</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="I563" t="inlineStr">
+        <is>
+          <t>internet</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="I564" t="inlineStr">
+        <is>
+          <t>industrial visit</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="I565" t="inlineStr">
+        <is>
+          <t>bsnl</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="I566" t="inlineStr">
+        <is>
+          <t>chennai</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>